<commit_message>
finished the Items + added documents for the "Expertenrunde"
</commit_message>
<xml_diff>
--- a/Items Monstera.xlsx
+++ b/Items Monstera.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f9055710c5e3c483/Documents/Monstera/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="145" documentId="8_{8E6482B4-6D64-4E3A-AAE1-966F7251B445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62E9CE6A-97C4-4DAD-B638-030755963A8B}"/>
+  <xr:revisionPtr revIDLastSave="334" documentId="8_{8E6482B4-6D64-4E3A-AAE1-966F7251B445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{641036D4-F5F8-49D7-85DC-8DC9BCCD0BC0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A2520A3A-2C53-47A9-9216-2F4E40D570BD}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1508" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1599" uniqueCount="277">
   <si>
     <t>Item</t>
   </si>
@@ -685,9 +685,6 @@
     <t>hat daher mehr Corona-Tote als andere Länder.</t>
   </si>
   <si>
-    <t>sagt trotzdem zu, weil er besser werden will.</t>
-  </si>
-  <si>
     <t xml:space="preserve">hat schlecht abgeschnitten. </t>
   </si>
   <si>
@@ -734,13 +731,160 @@
   </si>
   <si>
     <t xml:space="preserve">springt sein Auto nicht an. </t>
+  </si>
+  <si>
+    <t>wird der Traum wahr.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wird der Traum wahr. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">werden nicht gefragt. </t>
+  </si>
+  <si>
+    <t>sind die neuen Strategie Papiere erhältlich.</t>
+  </si>
+  <si>
+    <t>hat sehr viele Corona.Tote</t>
+  </si>
+  <si>
+    <t>hat daher mehr Corona.Tote als andere Länder</t>
+  </si>
+  <si>
+    <t>folgt sein Hund Max aufs Wort.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">müssen beide nochmal alles geben. </t>
+  </si>
+  <si>
+    <t>müssen beide nochmal alles geben.</t>
+  </si>
+  <si>
+    <t>hat jetzt keine angst mehr vor dem Doktor.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">muss mehr auf Ihre Ausgaben achten. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sollte es mit ihrer Bankausbildung besser wissen. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">hatte dieses Mal die beste Note. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">vergisst diesen wichtigen Termin und hat sich einen Tag frei genommen. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">nimmt es Kevin besonders genau. </t>
+  </si>
+  <si>
+    <t>nur noch abwarten und dann ein Ticket ergattern!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kommt die Pflegehilfe. Allerdings etwas früher, damit sie rechtzeitig los kann. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">trifft sie in der Stadt eine alte Freundin. </t>
+  </si>
+  <si>
+    <t>bringt er ihr einen prächtigen Strauß mit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">erfährt, dass sie die Firma verlassen muss. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">wird nachts von einem Unbekannten zerkratzt. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sind die Auftragsbücher voll und wird ihren Urlaub abgelehnt. </t>
+  </si>
+  <si>
+    <t>macht sich große Sorgen vor diesem Gespräch.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bereitet das Gespräch gut vor. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ist weiß und wird dadurch schneller dreckig. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">hat über 40.000 Euro gekostet. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">profitieren unter dem Strich gar nicht von diesem Angebot. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">holt er sich erst noch einen Kaffee bei Starbucks. </t>
+  </si>
+  <si>
+    <t>verschießt all seine Schüsse.</t>
+  </si>
+  <si>
+    <t>macht sich überhaupt keine Gedanken.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">erfährt sie, dass die Kundin mit der Zusammenarbeit einverstanden ist. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">weiß, dass sie gekündigt werden könnte. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">fällt durch. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">wird die Inspektion leider verschoben. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">gelingt Kevin vor lauter Nervosität nichts. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">hört ihm der Hund überhaupt nicht zu. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ist das Wetter noch so schlecht. Die Woche darauf wird es besser. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ist sehr wertvoll. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">hat absolut keine Lust auf Golf. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">hat keine Ahnung wie man Golf spielt. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">gewinnt das Spiel. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ist momentan in Topform. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">setzt sich sehr unter Druck. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">hat noch nie ein Spiel gespielt. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ist Janina aber immer noch sehr nervös. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">vergisst er ihr Blumen mitzunehmen. </t>
+  </si>
+  <si>
+    <t>hat soviel Erfahrung!</t>
+  </si>
+  <si>
+    <t>wacht sie auf und sieht sie nichts mehr! So kann sich nicht autofahren.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in der ersten Woche bekommt man nämlich eine exklusive ABBA-Poster beim Konzertbesuch. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -766,6 +910,12 @@
     <font>
       <sz val="11"/>
       <color theme="0" tint="-0.14999847407452621"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -852,7 +1002,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -894,6 +1044,34 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1273,10 +1451,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F935875C-1217-4EF1-B3EC-ADF1C73B1192}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:M563"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" topLeftCell="E160" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L170" sqref="L170:L172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1292,7 +1473,7 @@
     <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="76" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="85.85546875" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1333,7 +1514,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1346,7 +1527,7 @@
       <c r="D2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="57" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -1368,7 +1549,7 @@
         <v>1</v>
       </c>
       <c r="L2" s="11" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1405,7 +1586,9 @@
       <c r="K3" s="5">
         <v>2</v>
       </c>
-      <c r="L3" s="12"/>
+      <c r="L3" s="12" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="4" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
@@ -1442,10 +1625,10 @@
         <v>3</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -1458,7 +1641,7 @@
       <c r="D5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="58" t="s">
         <v>24</v>
       </c>
       <c r="F5" s="6" t="s">
@@ -1480,7 +1663,7 @@
         <v>4</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1517,7 +1700,9 @@
       <c r="K6" s="5">
         <v>5</v>
       </c>
-      <c r="L6" s="12"/>
+      <c r="L6" s="12" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="7" spans="1:12" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
@@ -1554,7 +1739,7 @@
         <v>6</v>
       </c>
       <c r="L7" s="13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="8" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -1773,7 +1958,7 @@
       </c>
       <c r="L13" s="28"/>
     </row>
-    <row r="14" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>3</v>
       </c>
@@ -1786,7 +1971,7 @@
       <c r="D14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="57" t="s">
         <v>31</v>
       </c>
       <c r="F14" s="3" t="s">
@@ -1807,7 +1992,9 @@
       <c r="K14" s="2">
         <v>3</v>
       </c>
-      <c r="L14" s="11"/>
+      <c r="L14" s="11" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="15" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
@@ -1843,7 +2030,9 @@
       <c r="K15" s="5">
         <v>4</v>
       </c>
-      <c r="L15" s="12"/>
+      <c r="L15" s="12" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="16" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
@@ -1879,9 +2068,11 @@
       <c r="K16" s="5">
         <v>5</v>
       </c>
-      <c r="L16" s="12"/>
-    </row>
-    <row r="17" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L16" s="12" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>3</v>
       </c>
@@ -1894,7 +2085,7 @@
       <c r="D17" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="58" t="s">
         <v>35</v>
       </c>
       <c r="F17" s="6" t="s">
@@ -1915,7 +2106,9 @@
       <c r="K17" s="5">
         <v>6</v>
       </c>
-      <c r="L17" s="12"/>
+      <c r="L17" s="12" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="18" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
@@ -1951,7 +2144,9 @@
       <c r="K18" s="5">
         <v>1</v>
       </c>
-      <c r="L18" s="12"/>
+      <c r="L18" s="12" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="19" spans="1:12" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7">
@@ -1987,9 +2182,11 @@
       <c r="K19" s="8">
         <v>2</v>
       </c>
-      <c r="L19" s="13"/>
-    </row>
-    <row r="20" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L19" s="13" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>4</v>
       </c>
@@ -2002,7 +2199,7 @@
       <c r="D20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="57" t="s">
         <v>37</v>
       </c>
       <c r="F20" s="3" t="s">
@@ -2024,7 +2221,7 @@
         <v>4</v>
       </c>
       <c r="L20" s="11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="21" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2061,7 +2258,9 @@
       <c r="K21" s="5">
         <v>5</v>
       </c>
-      <c r="L21" s="12"/>
+      <c r="L21" s="12" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="22" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
@@ -2098,10 +2297,10 @@
         <v>6</v>
       </c>
       <c r="L22" s="12" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>4</v>
       </c>
@@ -2114,7 +2313,7 @@
       <c r="D23" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="58" t="s">
         <v>44</v>
       </c>
       <c r="F23" s="6" t="s">
@@ -2136,7 +2335,7 @@
         <v>1</v>
       </c>
       <c r="L23" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="24" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2173,7 +2372,9 @@
       <c r="K24" s="5">
         <v>2</v>
       </c>
-      <c r="L24" s="12"/>
+      <c r="L24" s="12" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="25" spans="1:12" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
@@ -2210,10 +2411,10 @@
         <v>3</v>
       </c>
       <c r="L25" s="12" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>5</v>
       </c>
@@ -2226,7 +2427,7 @@
       <c r="D26" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="57" t="s">
         <v>45</v>
       </c>
       <c r="F26" s="3" t="s">
@@ -2247,7 +2448,9 @@
       <c r="K26" s="2">
         <v>5</v>
       </c>
-      <c r="L26" s="11"/>
+      <c r="L26" s="11" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="27" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
@@ -2283,7 +2486,9 @@
       <c r="K27" s="5">
         <v>6</v>
       </c>
-      <c r="L27" s="12"/>
+      <c r="L27" s="12" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="28" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
@@ -2323,7 +2528,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="29" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>5</v>
       </c>
@@ -2336,7 +2541,7 @@
       <c r="D29" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="E29" s="58" t="s">
         <v>50</v>
       </c>
       <c r="F29" s="6" t="s">
@@ -2357,7 +2562,9 @@
       <c r="K29" s="5">
         <v>2</v>
       </c>
-      <c r="L29" s="12"/>
+      <c r="L29" s="12" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="30" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
@@ -2393,7 +2600,9 @@
       <c r="K30" s="5">
         <v>3</v>
       </c>
-      <c r="L30" s="12"/>
+      <c r="L30" s="12" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="31" spans="1:12" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="7">
@@ -2649,7 +2858,7 @@
       </c>
       <c r="L37" s="28"/>
     </row>
-    <row r="38" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>7</v>
       </c>
@@ -2662,7 +2871,7 @@
       <c r="D38" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="E38" s="57" t="s">
         <v>57</v>
       </c>
       <c r="F38" s="3" t="s">
@@ -2683,7 +2892,9 @@
       <c r="K38" s="2">
         <v>1</v>
       </c>
-      <c r="L38" s="11"/>
+      <c r="L38" s="11" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="39" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
@@ -2720,7 +2931,7 @@
         <v>2</v>
       </c>
       <c r="L39" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="40" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2761,7 +2972,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="41" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>7</v>
       </c>
@@ -2774,7 +2985,7 @@
       <c r="D41" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E41" s="6" t="s">
+      <c r="E41" s="58" t="s">
         <v>65</v>
       </c>
       <c r="F41" s="6" t="s">
@@ -2795,7 +3006,9 @@
       <c r="K41" s="5">
         <v>4</v>
       </c>
-      <c r="L41" s="12"/>
+      <c r="L41" s="12" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="42" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
@@ -2832,7 +3045,7 @@
         <v>5</v>
       </c>
       <c r="L42" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="43" spans="1:12" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2873,7 +3086,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="44" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>8</v>
       </c>
@@ -2886,7 +3099,7 @@
       <c r="D44" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="E44" s="57" t="s">
         <v>66</v>
       </c>
       <c r="F44" s="3" t="s">
@@ -2908,7 +3121,7 @@
         <v>2</v>
       </c>
       <c r="L44" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="45" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2945,7 +3158,9 @@
       <c r="K45" s="5">
         <v>3</v>
       </c>
-      <c r="L45" s="12"/>
+      <c r="L45" s="12" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="46" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
@@ -2985,7 +3200,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="47" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>8</v>
       </c>
@@ -2998,7 +3213,7 @@
       <c r="D47" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E47" s="6" t="s">
+      <c r="E47" s="58" t="s">
         <v>72</v>
       </c>
       <c r="F47" s="6" t="s">
@@ -3020,7 +3235,7 @@
         <v>5</v>
       </c>
       <c r="L47" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="48" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3057,7 +3272,9 @@
       <c r="K48" s="5">
         <v>6</v>
       </c>
-      <c r="L48" s="12"/>
+      <c r="L48" s="12" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="49" spans="1:12" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="7">
@@ -3093,11 +3310,11 @@
       <c r="K49" s="8">
         <v>1</v>
       </c>
-      <c r="L49" s="12" t="s">
+      <c r="L49" s="13" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="50" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>9</v>
       </c>
@@ -3110,7 +3327,7 @@
       <c r="D50" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E50" s="3" t="s">
+      <c r="E50" s="57" t="s">
         <v>73</v>
       </c>
       <c r="F50" s="3" t="s">
@@ -3132,7 +3349,7 @@
         <v>3</v>
       </c>
       <c r="L50" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="51" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3207,7 +3424,9 @@
       <c r="K52" s="5">
         <v>5</v>
       </c>
-      <c r="L52" s="12"/>
+      <c r="L52" s="12" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="53" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
@@ -3244,7 +3463,7 @@
         <v>6</v>
       </c>
       <c r="L53" s="12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="54" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3319,9 +3538,11 @@
       <c r="K55" s="8">
         <v>2</v>
       </c>
-      <c r="L55" s="12"/>
-    </row>
-    <row r="56" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L55" s="13" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>10</v>
       </c>
@@ -3334,7 +3555,7 @@
       <c r="D56" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E56" s="3" t="s">
+      <c r="E56" s="57" t="s">
         <v>80</v>
       </c>
       <c r="F56" s="3" t="s">
@@ -3355,7 +3576,9 @@
       <c r="K56" s="2">
         <v>4</v>
       </c>
-      <c r="L56" s="12"/>
+      <c r="L56" s="12" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="57" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
@@ -3391,7 +3614,9 @@
       <c r="K57" s="5">
         <v>5</v>
       </c>
-      <c r="L57" s="12"/>
+      <c r="L57" s="12" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="58" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
@@ -3428,10 +3653,10 @@
         <v>6</v>
       </c>
       <c r="L58" s="12" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>10</v>
       </c>
@@ -3444,7 +3669,7 @@
       <c r="D59" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E59" s="6" t="s">
+      <c r="E59" s="58" t="s">
         <v>85</v>
       </c>
       <c r="F59" s="6" t="s">
@@ -3465,7 +3690,9 @@
       <c r="K59" s="5">
         <v>1</v>
       </c>
-      <c r="L59" s="12"/>
+      <c r="L59" s="12" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="60" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
@@ -3501,7 +3728,9 @@
       <c r="K60" s="5">
         <v>2</v>
       </c>
-      <c r="L60" s="12"/>
+      <c r="L60" s="12" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="61" spans="1:12" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="7">
@@ -3538,10 +3767,10 @@
         <v>3</v>
       </c>
       <c r="L61" s="13" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>11</v>
       </c>
@@ -3554,7 +3783,7 @@
       <c r="D62" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E62" s="3" t="s">
+      <c r="E62" s="57" t="s">
         <v>86</v>
       </c>
       <c r="F62" s="3" t="s">
@@ -3575,7 +3804,9 @@
       <c r="K62" s="2">
         <v>5</v>
       </c>
-      <c r="L62" s="11"/>
+      <c r="L62" s="11" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="63" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
@@ -3612,7 +3843,7 @@
         <v>6</v>
       </c>
       <c r="L63" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="64" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3649,9 +3880,11 @@
       <c r="K64" s="5">
         <v>1</v>
       </c>
-      <c r="L64" s="12"/>
-    </row>
-    <row r="65" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L64" s="12" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>11</v>
       </c>
@@ -3664,7 +3897,7 @@
       <c r="D65" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E65" s="6" t="s">
+      <c r="E65" s="58" t="s">
         <v>92</v>
       </c>
       <c r="F65" s="6" t="s">
@@ -3685,7 +3918,9 @@
       <c r="K65" s="5">
         <v>2</v>
       </c>
-      <c r="L65" s="12"/>
+      <c r="L65" s="12" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="66" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
@@ -3722,7 +3957,7 @@
         <v>3</v>
       </c>
       <c r="L66" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="67" spans="1:12" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3759,9 +3994,11 @@
       <c r="K67" s="8">
         <v>4</v>
       </c>
-      <c r="L67" s="13"/>
-    </row>
-    <row r="68" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L67" s="13" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>12</v>
       </c>
@@ -3774,7 +4011,7 @@
       <c r="D68" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E68" s="3" t="s">
+      <c r="E68" s="57" t="s">
         <v>93</v>
       </c>
       <c r="F68" s="3" t="s">
@@ -3795,7 +4032,9 @@
       <c r="K68" s="2">
         <v>6</v>
       </c>
-      <c r="L68" s="11"/>
+      <c r="L68" s="11" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="69" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
@@ -3831,7 +4070,9 @@
       <c r="K69" s="5">
         <v>1</v>
       </c>
-      <c r="L69" s="12"/>
+      <c r="L69" s="12" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="70" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
@@ -3867,9 +4108,11 @@
       <c r="K70" s="5">
         <v>2</v>
       </c>
-      <c r="L70" s="12"/>
-    </row>
-    <row r="71" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L70" s="12" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
         <v>12</v>
       </c>
@@ -3882,7 +4125,7 @@
       <c r="D71" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E71" s="6" t="s">
+      <c r="E71" s="58" t="s">
         <v>97</v>
       </c>
       <c r="F71" s="6" t="s">
@@ -3903,7 +4146,9 @@
       <c r="K71" s="5">
         <v>3</v>
       </c>
-      <c r="L71" s="12"/>
+      <c r="L71" s="12" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="72" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
@@ -3939,7 +4184,9 @@
       <c r="K72" s="5">
         <v>4</v>
       </c>
-      <c r="L72" s="12"/>
+      <c r="L72" s="12" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="73" spans="1:12" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="7">
@@ -3975,227 +4222,233 @@
       <c r="K73" s="8">
         <v>5</v>
       </c>
-      <c r="L73" s="13"/>
-    </row>
-    <row r="74" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="1">
+      <c r="L73" s="13" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="29">
         <v>13</v>
       </c>
-      <c r="B74" s="2">
+      <c r="B74" s="30">
         <v>1</v>
       </c>
-      <c r="C74" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D74" s="3" t="s">
+      <c r="C74" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D74" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E74" s="3" t="s">
+      <c r="E74" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="F74" s="3" t="s">
+      <c r="F74" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="G74" s="3" t="s">
+      <c r="G74" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="H74" s="3" t="s">
+      <c r="H74" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="I74" s="3" t="s">
+      <c r="I74" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="J74" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K74" s="2">
+      <c r="J74" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="K74" s="30">
         <v>1</v>
       </c>
-      <c r="L74" s="11"/>
-    </row>
-    <row r="75" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="4">
+      <c r="L74" s="53"/>
+    </row>
+    <row r="75" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="33">
         <v>13</v>
       </c>
-      <c r="B75" s="5">
+      <c r="B75" s="34">
         <v>2</v>
       </c>
-      <c r="C75" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D75" s="6" t="s">
+      <c r="C75" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="D75" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="E75" s="6" t="s">
+      <c r="E75" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="F75" s="6" t="s">
+      <c r="F75" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="G75" s="6" t="s">
+      <c r="G75" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="H75" s="6" t="s">
+      <c r="H75" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="I75" s="6" t="s">
+      <c r="I75" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="J75" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K75" s="5">
+      <c r="J75" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="K75" s="34">
         <v>2</v>
       </c>
-      <c r="L75" s="12"/>
-    </row>
-    <row r="76" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="4">
+      <c r="L75" s="54"/>
+    </row>
+    <row r="76" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="33">
         <v>13</v>
       </c>
-      <c r="B76" s="5">
+      <c r="B76" s="34">
         <v>3</v>
       </c>
-      <c r="C76" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D76" s="6" t="s">
+      <c r="C76" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="D76" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="E76" s="6" t="s">
+      <c r="E76" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="F76" s="6" t="s">
+      <c r="F76" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="G76" s="6" t="s">
+      <c r="G76" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="H76" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I76" s="6" t="s">
+      <c r="H76" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="I76" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="J76" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K76" s="5">
+      <c r="J76" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="K76" s="34">
         <v>3</v>
       </c>
-      <c r="L76" s="12" t="s">
+      <c r="L76" s="54" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="77" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="4">
+    <row r="77" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="33">
         <v>13</v>
       </c>
-      <c r="B77" s="5">
+      <c r="B77" s="34">
         <v>4</v>
       </c>
-      <c r="C77" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D77" s="6" t="s">
+      <c r="C77" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="D77" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="E77" s="6" t="s">
+      <c r="E77" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="F77" s="6" t="s">
+      <c r="F77" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="G77" s="6" t="s">
+      <c r="G77" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="H77" s="6" t="s">
+      <c r="H77" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="I77" s="6" t="s">
+      <c r="I77" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="J77" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K77" s="5">
+      <c r="J77" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="K77" s="34">
         <v>4</v>
       </c>
-      <c r="L77" s="12"/>
-    </row>
-    <row r="78" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="4">
+      <c r="L77" s="54"/>
+    </row>
+    <row r="78" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="33">
         <v>13</v>
       </c>
-      <c r="B78" s="5">
+      <c r="B78" s="34">
         <v>5</v>
       </c>
-      <c r="C78" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D78" s="6" t="s">
+      <c r="C78" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="D78" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="E78" s="6" t="s">
+      <c r="E78" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="F78" s="6" t="s">
+      <c r="F78" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="G78" s="6" t="s">
+      <c r="G78" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="H78" s="6" t="s">
+      <c r="H78" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="I78" s="6" t="s">
+      <c r="I78" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="J78" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K78" s="5">
+      <c r="J78" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="K78" s="34">
         <v>5</v>
       </c>
-      <c r="L78" s="12"/>
-    </row>
-    <row r="79" spans="1:12" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="7">
+      <c r="L78" s="54" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" s="38" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="37">
         <v>13</v>
       </c>
-      <c r="B79" s="8">
+      <c r="B79" s="38">
         <v>6</v>
       </c>
-      <c r="C79" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D79" s="9" t="s">
+      <c r="C79" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="D79" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="E79" s="9" t="s">
+      <c r="E79" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="F79" s="9" t="s">
+      <c r="F79" s="39" t="s">
         <v>100</v>
       </c>
-      <c r="G79" s="9" t="s">
+      <c r="G79" s="39" t="s">
         <v>100</v>
       </c>
-      <c r="H79" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="I79" s="9" t="s">
+      <c r="H79" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="I79" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="J79" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="K79" s="8">
+      <c r="J79" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="K79" s="38">
         <v>6</v>
       </c>
-      <c r="L79" s="13"/>
-    </row>
-    <row r="80" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L79" s="55" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>14</v>
       </c>
@@ -4208,7 +4461,7 @@
       <c r="D80" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E80" s="3" t="s">
+      <c r="E80" s="57" t="s">
         <v>103</v>
       </c>
       <c r="F80" s="3" t="s">
@@ -4229,7 +4482,9 @@
       <c r="K80" s="2">
         <v>2</v>
       </c>
-      <c r="L80" s="11"/>
+      <c r="L80" s="11" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="81" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
@@ -4265,7 +4520,9 @@
       <c r="K81" s="5">
         <v>3</v>
       </c>
-      <c r="L81" s="12"/>
+      <c r="L81" s="12" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="82" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
@@ -4305,7 +4562,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="83" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
         <v>14</v>
       </c>
@@ -4318,7 +4575,7 @@
       <c r="D83" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E83" s="6" t="s">
+      <c r="E83" s="58" t="s">
         <v>107</v>
       </c>
       <c r="F83" s="6" t="s">
@@ -4339,7 +4596,9 @@
       <c r="K83" s="5">
         <v>5</v>
       </c>
-      <c r="L83" s="12"/>
+      <c r="L83" s="12" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="84" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
@@ -4375,7 +4634,9 @@
       <c r="K84" s="5">
         <v>6</v>
       </c>
-      <c r="L84" s="12"/>
+      <c r="L84" s="12" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="85" spans="1:12" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="7">
@@ -4415,7 +4676,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="86" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>15</v>
       </c>
@@ -4428,7 +4689,7 @@
       <c r="D86" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E86" s="3" t="s">
+      <c r="E86" s="57" t="s">
         <v>108</v>
       </c>
       <c r="F86" s="3" t="s">
@@ -4449,7 +4710,9 @@
       <c r="K86" s="2">
         <v>3</v>
       </c>
-      <c r="L86" s="11"/>
+      <c r="L86" s="11" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="87" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
@@ -4485,7 +4748,9 @@
       <c r="K87" s="5">
         <v>4</v>
       </c>
-      <c r="L87" s="12"/>
+      <c r="L87" s="12" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="88" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="4">
@@ -4521,9 +4786,11 @@
       <c r="K88" s="5">
         <v>5</v>
       </c>
-      <c r="L88" s="12"/>
-    </row>
-    <row r="89" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L88" s="12" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
         <v>15</v>
       </c>
@@ -4536,7 +4803,7 @@
       <c r="D89" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E89" s="6" t="s">
+      <c r="E89" s="58" t="s">
         <v>114</v>
       </c>
       <c r="F89" s="6" t="s">
@@ -4557,7 +4824,9 @@
       <c r="K89" s="5">
         <v>6</v>
       </c>
-      <c r="L89" s="12"/>
+      <c r="L89" s="12" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="90" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="4">
@@ -4593,7 +4862,9 @@
       <c r="K90" s="5">
         <v>1</v>
       </c>
-      <c r="L90" s="12"/>
+      <c r="L90" s="12" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="91" spans="1:12" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="7">
@@ -4629,225 +4900,239 @@
       <c r="K91" s="8">
         <v>2</v>
       </c>
-      <c r="L91" s="13"/>
-    </row>
-    <row r="92" spans="1:12" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="29">
+      <c r="L91" s="12" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" s="42" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A92" s="41">
         <v>16</v>
       </c>
-      <c r="B92" s="30">
+      <c r="B92" s="42">
         <v>1</v>
       </c>
-      <c r="C92" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="D92" s="31" t="s">
+      <c r="C92" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="D92" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="E92" s="31" t="s">
+      <c r="E92" s="59" t="s">
         <v>115</v>
       </c>
-      <c r="F92" s="31" t="s">
+      <c r="F92" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="G92" s="31" t="s">
+      <c r="G92" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="H92" s="31" t="s">
+      <c r="H92" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="I92" s="31" t="s">
+      <c r="I92" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="J92" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="K92" s="30">
+      <c r="J92" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="K92" s="42">
         <v>4</v>
       </c>
-      <c r="L92" s="32"/>
-    </row>
-    <row r="93" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="33">
+      <c r="L92" s="44" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="45">
         <v>16</v>
       </c>
-      <c r="B93" s="34">
+      <c r="B93" s="46">
         <v>2</v>
       </c>
-      <c r="C93" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="D93" s="35" t="s">
+      <c r="C93" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="D93" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="E93" s="35" t="s">
+      <c r="E93" s="47" t="s">
         <v>115</v>
       </c>
-      <c r="F93" s="35" t="s">
+      <c r="F93" s="47" t="s">
         <v>118</v>
       </c>
-      <c r="G93" s="35" t="s">
+      <c r="G93" s="47" t="s">
         <v>117</v>
       </c>
-      <c r="H93" s="35" t="s">
+      <c r="H93" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="I93" s="35" t="s">
+      <c r="I93" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="J93" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="K93" s="34">
+      <c r="J93" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="K93" s="46">
         <v>5</v>
       </c>
-      <c r="L93" s="36"/>
-    </row>
-    <row r="94" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="33">
+      <c r="L93" s="48" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="45">
         <v>16</v>
       </c>
-      <c r="B94" s="34">
+      <c r="B94" s="46">
         <v>3</v>
       </c>
-      <c r="C94" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="D94" s="35" t="s">
+      <c r="C94" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="D94" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="E94" s="35" t="s">
+      <c r="E94" s="47" t="s">
         <v>115</v>
       </c>
-      <c r="F94" s="35" t="s">
+      <c r="F94" s="47" t="s">
         <v>119</v>
       </c>
-      <c r="G94" s="35" t="s">
+      <c r="G94" s="47" t="s">
         <v>117</v>
       </c>
-      <c r="H94" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="I94" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="J94" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="K94" s="34">
+      <c r="H94" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="I94" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="J94" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="K94" s="46">
         <v>6</v>
       </c>
-      <c r="L94" s="36"/>
-    </row>
-    <row r="95" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="33">
+      <c r="L94" s="48" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" s="46" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A95" s="45">
         <v>16</v>
       </c>
-      <c r="B95" s="34">
+      <c r="B95" s="46">
         <v>4</v>
       </c>
-      <c r="C95" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="D95" s="35" t="s">
+      <c r="C95" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="D95" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="E95" s="35" t="s">
+      <c r="E95" s="60" t="s">
         <v>120</v>
       </c>
-      <c r="F95" s="35" t="s">
+      <c r="F95" s="47" t="s">
         <v>116</v>
       </c>
-      <c r="G95" s="35" t="s">
+      <c r="G95" s="47" t="s">
         <v>117</v>
       </c>
-      <c r="H95" s="35" t="s">
+      <c r="H95" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="I95" s="35" t="s">
+      <c r="I95" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="J95" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="K95" s="34">
+      <c r="J95" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="K95" s="46">
         <v>1</v>
       </c>
-      <c r="L95" s="36"/>
-    </row>
-    <row r="96" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="33">
+      <c r="L95" s="48" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="45">
         <v>16</v>
       </c>
-      <c r="B96" s="34">
+      <c r="B96" s="46">
         <v>5</v>
       </c>
-      <c r="C96" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="D96" s="35" t="s">
+      <c r="C96" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="D96" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="E96" s="35" t="s">
+      <c r="E96" s="47" t="s">
         <v>120</v>
       </c>
-      <c r="F96" s="35" t="s">
+      <c r="F96" s="47" t="s">
         <v>118</v>
       </c>
-      <c r="G96" s="35" t="s">
+      <c r="G96" s="47" t="s">
         <v>117</v>
       </c>
-      <c r="H96" s="35" t="s">
+      <c r="H96" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="I96" s="35" t="s">
+      <c r="I96" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="J96" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="K96" s="34">
+      <c r="J96" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="K96" s="46">
         <v>2</v>
       </c>
-      <c r="L96" s="36"/>
-    </row>
-    <row r="97" spans="1:12" s="38" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="37">
+      <c r="L96" s="48" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" s="50" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="49">
         <v>16</v>
       </c>
-      <c r="B97" s="38">
+      <c r="B97" s="50">
         <v>6</v>
       </c>
-      <c r="C97" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="D97" s="39" t="s">
+      <c r="C97" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="D97" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="E97" s="39" t="s">
+      <c r="E97" s="51" t="s">
         <v>120</v>
       </c>
-      <c r="F97" s="39" t="s">
+      <c r="F97" s="51" t="s">
         <v>119</v>
       </c>
-      <c r="G97" s="39" t="s">
+      <c r="G97" s="51" t="s">
         <v>117</v>
       </c>
-      <c r="H97" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="I97" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="J97" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="K97" s="38">
+      <c r="H97" s="51" t="s">
+        <v>22</v>
+      </c>
+      <c r="I97" s="51" t="s">
+        <v>22</v>
+      </c>
+      <c r="J97" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="K97" s="50">
         <v>3</v>
       </c>
-      <c r="L97" s="40"/>
-    </row>
-    <row r="98" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L97" s="52" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>17</v>
       </c>
@@ -4860,7 +5145,7 @@
       <c r="D98" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E98" s="3" t="s">
+      <c r="E98" s="57" t="s">
         <v>121</v>
       </c>
       <c r="F98" s="3" t="s">
@@ -4881,7 +5166,9 @@
       <c r="K98" s="2">
         <v>5</v>
       </c>
-      <c r="L98" s="11"/>
+      <c r="L98" s="11" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="99" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="4">
@@ -4959,7 +5246,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="101" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A101" s="4">
         <v>17</v>
       </c>
@@ -4972,7 +5259,7 @@
       <c r="D101" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E101" s="6" t="s">
+      <c r="E101" s="58" t="s">
         <v>126</v>
       </c>
       <c r="F101" s="6" t="s">
@@ -4993,7 +5280,9 @@
       <c r="K101" s="5">
         <v>2</v>
       </c>
-      <c r="L101" s="12"/>
+      <c r="L101" s="12" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="102" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="4">
@@ -5067,11 +5356,11 @@
       <c r="K103" s="8">
         <v>4</v>
       </c>
-      <c r="L103" s="12" t="s">
+      <c r="L103" s="13" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="104" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>18</v>
       </c>
@@ -5084,7 +5373,7 @@
       <c r="D104" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E104" s="3" t="s">
+      <c r="E104" s="57" t="s">
         <v>127</v>
       </c>
       <c r="F104" s="3" t="s">
@@ -5106,7 +5395,7 @@
         <v>6</v>
       </c>
       <c r="L104" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="105" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -5181,9 +5470,11 @@
       <c r="K106" s="5">
         <v>2</v>
       </c>
-      <c r="L106" s="14"/>
-    </row>
-    <row r="107" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L106" s="14" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A107" s="4">
         <v>18</v>
       </c>
@@ -5196,7 +5487,7 @@
       <c r="D107" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E107" s="6" t="s">
+      <c r="E107" s="58" t="s">
         <v>132</v>
       </c>
       <c r="F107" s="6" t="s">
@@ -5218,7 +5509,7 @@
         <v>3</v>
       </c>
       <c r="L107" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="108" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -5293,9 +5584,11 @@
       <c r="K109" s="8">
         <v>5</v>
       </c>
-      <c r="L109" s="14"/>
-    </row>
-    <row r="110" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L109" s="56" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>19</v>
       </c>
@@ -5308,7 +5601,7 @@
       <c r="D110" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E110" s="3" t="s">
+      <c r="E110" s="57" t="s">
         <v>133</v>
       </c>
       <c r="F110" s="3" t="s">
@@ -5329,7 +5622,9 @@
       <c r="K110" s="2">
         <v>1</v>
       </c>
-      <c r="L110" s="12"/>
+      <c r="L110" s="12" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="111" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="4">
@@ -5365,7 +5660,9 @@
       <c r="K111" s="5">
         <v>2</v>
       </c>
-      <c r="L111" s="12"/>
+      <c r="L111" s="12" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="112" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="4">
@@ -5402,10 +5699,10 @@
         <v>3</v>
       </c>
       <c r="L112" s="12" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="113" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" s="4">
         <v>19</v>
       </c>
@@ -5418,7 +5715,7 @@
       <c r="D113" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E113" s="6" t="s">
+      <c r="E113" s="58" t="s">
         <v>138</v>
       </c>
       <c r="F113" s="6" t="s">
@@ -5439,7 +5736,9 @@
       <c r="K113" s="5">
         <v>4</v>
       </c>
-      <c r="L113" s="12"/>
+      <c r="L113" s="12" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="114" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="4">
@@ -5475,7 +5774,9 @@
       <c r="K114" s="5">
         <v>5</v>
       </c>
-      <c r="L114" s="12"/>
+      <c r="L114" s="12" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="115" spans="1:12" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="7">
@@ -5511,9 +5812,11 @@
       <c r="K115" s="8">
         <v>6</v>
       </c>
-      <c r="L115" s="13"/>
-    </row>
-    <row r="116" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L115" s="13" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>20</v>
       </c>
@@ -5526,7 +5829,7 @@
       <c r="D116" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E116" s="3" t="s">
+      <c r="E116" s="57" t="s">
         <v>139</v>
       </c>
       <c r="F116" s="3" t="s">
@@ -5548,7 +5851,7 @@
         <v>2</v>
       </c>
       <c r="L116" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="117" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -5586,7 +5889,7 @@
         <v>3</v>
       </c>
       <c r="L117" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="118" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -5627,7 +5930,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="119" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A119" s="4">
         <v>20</v>
       </c>
@@ -5640,7 +5943,7 @@
       <c r="D119" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E119" s="6" t="s">
+      <c r="E119" s="58" t="s">
         <v>144</v>
       </c>
       <c r="F119" s="6" t="s">
@@ -5662,7 +5965,7 @@
         <v>5</v>
       </c>
       <c r="L119" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="120" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -5700,7 +6003,7 @@
         <v>6</v>
       </c>
       <c r="L120" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="121" spans="1:12" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5741,7 +6044,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="122" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>21</v>
       </c>
@@ -5754,7 +6057,7 @@
       <c r="D122" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E122" s="3" t="s">
+      <c r="E122" s="57" t="s">
         <v>145</v>
       </c>
       <c r="F122" s="3" t="s">
@@ -5775,7 +6078,9 @@
       <c r="K122" s="2">
         <v>3</v>
       </c>
-      <c r="L122" s="11"/>
+      <c r="L122" s="11" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="123" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="4">
@@ -5811,7 +6116,9 @@
       <c r="K123" s="5">
         <v>4</v>
       </c>
-      <c r="L123" s="12"/>
+      <c r="L123" s="12" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="124" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="4">
@@ -5847,9 +6154,11 @@
       <c r="K124" s="5">
         <v>5</v>
       </c>
-      <c r="L124" s="12"/>
-    </row>
-    <row r="125" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L124" s="12" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A125" s="4">
         <v>21</v>
       </c>
@@ -5862,7 +6171,7 @@
       <c r="D125" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E125" s="6" t="s">
+      <c r="E125" s="58" t="s">
         <v>149</v>
       </c>
       <c r="F125" s="6" t="s">
@@ -5883,7 +6192,9 @@
       <c r="K125" s="5">
         <v>6</v>
       </c>
-      <c r="L125" s="12"/>
+      <c r="L125" s="12" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="126" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="4">
@@ -5919,7 +6230,9 @@
       <c r="K126" s="5">
         <v>1</v>
       </c>
-      <c r="L126" s="12"/>
+      <c r="L126" s="12" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="127" spans="1:12" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="7">
@@ -5955,9 +6268,11 @@
       <c r="K127" s="8">
         <v>2</v>
       </c>
-      <c r="L127" s="13"/>
-    </row>
-    <row r="128" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L127" s="13" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>22</v>
       </c>
@@ -5970,7 +6285,7 @@
       <c r="D128" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E128" s="3" t="s">
+      <c r="E128" s="57" t="s">
         <v>150</v>
       </c>
       <c r="F128" s="3" t="s">
@@ -5991,7 +6306,9 @@
       <c r="K128" s="2">
         <v>4</v>
       </c>
-      <c r="L128" s="11"/>
+      <c r="L128" s="11" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="129" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="4">
@@ -6027,7 +6344,9 @@
       <c r="K129" s="5">
         <v>5</v>
       </c>
-      <c r="L129" s="12"/>
+      <c r="L129" s="12" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="130" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="4">
@@ -6064,10 +6383,10 @@
         <v>6</v>
       </c>
       <c r="L130" s="12" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="131" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A131" s="4">
         <v>22</v>
       </c>
@@ -6080,7 +6399,7 @@
       <c r="D131" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E131" s="6" t="s">
+      <c r="E131" s="58" t="s">
         <v>152</v>
       </c>
       <c r="F131" s="6" t="s">
@@ -6101,7 +6420,9 @@
       <c r="K131" s="5">
         <v>1</v>
       </c>
-      <c r="L131" s="12"/>
+      <c r="L131" s="12" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="132" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="4">
@@ -6137,7 +6458,9 @@
       <c r="K132" s="5">
         <v>2</v>
       </c>
-      <c r="L132" s="12"/>
+      <c r="L132" s="12" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="133" spans="1:12" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="7">
@@ -6174,10 +6497,10 @@
         <v>3</v>
       </c>
       <c r="L133" s="13" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="134" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>23</v>
       </c>
@@ -6190,7 +6513,7 @@
       <c r="D134" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E134" s="3" t="s">
+      <c r="E134" s="57" t="s">
         <v>153</v>
       </c>
       <c r="F134" s="3" t="s">
@@ -6211,7 +6534,9 @@
       <c r="K134" s="2">
         <v>5</v>
       </c>
-      <c r="L134" s="11"/>
+      <c r="L134" s="11" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="135" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="4">
@@ -6247,7 +6572,9 @@
       <c r="K135" s="5">
         <v>6</v>
       </c>
-      <c r="L135" s="12"/>
+      <c r="L135" s="12" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="136" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="4">
@@ -6287,7 +6614,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="137" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A137" s="4">
         <v>23</v>
       </c>
@@ -6300,7 +6627,7 @@
       <c r="D137" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E137" s="6" t="s">
+      <c r="E137" s="58" t="s">
         <v>158</v>
       </c>
       <c r="F137" s="6" t="s">
@@ -6321,7 +6648,9 @@
       <c r="K137" s="5">
         <v>2</v>
       </c>
-      <c r="L137" s="12"/>
+      <c r="L137" s="12" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="138" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="4">
@@ -6357,7 +6686,9 @@
       <c r="K138" s="5">
         <v>3</v>
       </c>
-      <c r="L138" s="12"/>
+      <c r="L138" s="12" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="139" spans="1:12" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="7">
@@ -6397,7 +6728,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="140" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>24</v>
       </c>
@@ -6410,7 +6741,7 @@
       <c r="D140" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E140" s="3" t="s">
+      <c r="E140" s="57" t="s">
         <v>159</v>
       </c>
       <c r="F140" s="3" t="s">
@@ -6431,7 +6762,9 @@
       <c r="K140" s="2">
         <v>6</v>
       </c>
-      <c r="L140" s="11"/>
+      <c r="L140" s="11" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="141" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="4">
@@ -6467,7 +6800,9 @@
       <c r="K141" s="5">
         <v>1</v>
       </c>
-      <c r="L141" s="12"/>
+      <c r="L141" s="12" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="142" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A142" s="4">
@@ -6503,9 +6838,11 @@
       <c r="K142" s="5">
         <v>2</v>
       </c>
-      <c r="L142" s="12"/>
-    </row>
-    <row r="143" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L142" s="12" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A143" s="4">
         <v>24</v>
       </c>
@@ -6518,7 +6855,7 @@
       <c r="D143" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E143" s="6" t="s">
+      <c r="E143" s="58" t="s">
         <v>164</v>
       </c>
       <c r="F143" s="6" t="s">
@@ -6539,7 +6876,9 @@
       <c r="K143" s="5">
         <v>3</v>
       </c>
-      <c r="L143" s="12"/>
+      <c r="L143" s="12" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="144" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="4">
@@ -6575,7 +6914,9 @@
       <c r="K144" s="5">
         <v>4</v>
       </c>
-      <c r="L144" s="12"/>
+      <c r="L144" s="12" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="145" spans="1:12" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="7">
@@ -6611,7 +6952,9 @@
       <c r="K145" s="8">
         <v>5</v>
       </c>
-      <c r="L145" s="13"/>
+      <c r="L145" s="12" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="146" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A146" s="17">
@@ -6829,7 +7172,7 @@
       </c>
       <c r="L151" s="28"/>
     </row>
-    <row r="152" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:12" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>26</v>
       </c>
@@ -6842,7 +7185,7 @@
       <c r="D152" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E152" s="3" t="s">
+      <c r="E152" s="57" t="s">
         <v>170</v>
       </c>
       <c r="F152" s="3" t="s">
@@ -6863,7 +7206,9 @@
       <c r="K152" s="2">
         <v>2</v>
       </c>
-      <c r="L152" s="11"/>
+      <c r="L152" s="11" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="153" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A153" s="4">
@@ -6900,7 +7245,7 @@
         <v>3</v>
       </c>
       <c r="L153" s="12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="154" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -6941,7 +7286,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="155" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:12" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A155" s="4">
         <v>26</v>
       </c>
@@ -6954,7 +7299,7 @@
       <c r="D155" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E155" s="6" t="s">
+      <c r="E155" s="58" t="s">
         <v>174</v>
       </c>
       <c r="F155" s="6" t="s">
@@ -6975,7 +7320,9 @@
       <c r="K155" s="5">
         <v>5</v>
       </c>
-      <c r="L155" s="12"/>
+      <c r="L155" s="12" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="156" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A156" s="4">
@@ -7012,7 +7359,7 @@
         <v>6</v>
       </c>
       <c r="L156" s="12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="157" spans="1:12" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7053,7 +7400,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="158" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:12" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>27</v>
       </c>
@@ -7066,7 +7413,7 @@
       <c r="D158" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E158" s="3" t="s">
+      <c r="E158" s="57" t="s">
         <v>175</v>
       </c>
       <c r="F158" s="3" t="s">
@@ -7088,7 +7435,7 @@
         <v>3</v>
       </c>
       <c r="L158" s="11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="159" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -7125,9 +7472,11 @@
       <c r="K159" s="5">
         <v>4</v>
       </c>
-      <c r="L159" s="12"/>
-    </row>
-    <row r="160" spans="1:12" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L159" s="12" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="160" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A160" s="4">
         <v>27</v>
       </c>
@@ -7161,9 +7510,11 @@
       <c r="K160" s="5">
         <v>5</v>
       </c>
-      <c r="L160" s="12"/>
-    </row>
-    <row r="161" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L160" s="12" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="161" spans="1:13" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A161" s="4">
         <v>27</v>
       </c>
@@ -7176,7 +7527,7 @@
       <c r="D161" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E161" s="6" t="s">
+      <c r="E161" s="58" t="s">
         <v>179</v>
       </c>
       <c r="F161" s="6" t="s">
@@ -7197,8 +7548,8 @@
       <c r="K161" s="5">
         <v>6</v>
       </c>
-      <c r="L161" s="11" t="s">
-        <v>221</v>
+      <c r="L161" s="12" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="162" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -7235,7 +7586,9 @@
       <c r="K162" s="5">
         <v>1</v>
       </c>
-      <c r="L162" s="12"/>
+      <c r="L162" s="12" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="163" spans="1:13" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="7">
@@ -7271,7 +7624,9 @@
       <c r="K163" s="8">
         <v>2</v>
       </c>
-      <c r="L163" s="13"/>
+      <c r="L163" s="13" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="164" spans="1:13" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A164" s="29">
@@ -7489,7 +7844,7 @@
       </c>
       <c r="L169" s="40"/>
     </row>
-    <row r="170" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:13" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>29</v>
       </c>
@@ -7502,7 +7857,7 @@
       <c r="D170" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E170" s="3" t="s">
+      <c r="E170" s="57" t="s">
         <v>186</v>
       </c>
       <c r="F170" s="3" t="s">
@@ -7523,7 +7878,9 @@
       <c r="K170" s="2">
         <v>5</v>
       </c>
-      <c r="L170" s="11"/>
+      <c r="L170" s="11" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="171" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A171" s="4">
@@ -7559,7 +7916,9 @@
       <c r="K171" s="5">
         <v>6</v>
       </c>
-      <c r="L171" s="12"/>
+      <c r="L171" s="12" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="172" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A172" s="4">
@@ -7599,7 +7958,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="173" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:13" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A173" s="4">
         <v>29</v>
       </c>
@@ -7612,7 +7971,7 @@
       <c r="D173" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E173" s="6" t="s">
+      <c r="E173" s="58" t="s">
         <v>191</v>
       </c>
       <c r="F173" s="6" t="s">
@@ -7633,7 +7992,9 @@
       <c r="K173" s="5">
         <v>2</v>
       </c>
-      <c r="L173" s="12"/>
+      <c r="L173" s="12" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="174" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A174" s="4">
@@ -7669,7 +8030,9 @@
       <c r="K174" s="5">
         <v>3</v>
       </c>
-      <c r="L174" s="12"/>
+      <c r="L174" s="12" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="175" spans="1:13" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="7">
@@ -9079,7 +9442,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="26" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>